<commit_message>
Updates version number of Form C
</commit_message>
<xml_diff>
--- a/Hluvukani_C_registrar_parcelas/Hluvukani_C_registrar_parcelas-media/Hluvukani_C_registrar_parcelas.xlsx
+++ b/Hluvukani_C_registrar_parcelas/Hluvukani_C_registrar_parcelas-media/Hluvukani_C_registrar_parcelas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\GitHub\hluvukani-odk-forms\Hluvukani_C_registrar_parcelas\Hluvukani_C_registrar_parcelas-media\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\projects\illovo\ODK Forms\hluvukani-odk-forms\Hluvukani_C_registrar_parcelas\Hluvukani_C_registrar_parcelas-media\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -5935,7 +5935,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5969,7 +5969,7 @@
         <v>408</v>
       </c>
       <c r="C2" s="8">
-        <v>201708151</v>
+        <v>201708152</v>
       </c>
       <c r="D2" s="67" t="s">
         <v>410</v>

</xml_diff>

<commit_message>
Corrects misspelled Manhica in CSV media file
</commit_message>
<xml_diff>
--- a/Hluvukani_C_registrar_parcelas/Hluvukani_C_registrar_parcelas-media/Hluvukani_C_registrar_parcelas.xlsx
+++ b/Hluvukani_C_registrar_parcelas/Hluvukani_C_registrar_parcelas-media/Hluvukani_C_registrar_parcelas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7380" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7380" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -2038,7 +2038,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2199,21 +2199,24 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="237">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2792,10 +2795,10 @@
   <dimension ref="A1:P76"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="L20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A24" sqref="A24"/>
+      <selection pane="bottomRight" activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3263,27 +3266,27 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="80" t="s">
+      <c r="A23" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="81" t="s">
+      <c r="B23" s="80" t="s">
         <v>489</v>
       </c>
-      <c r="C23" s="80" t="s">
+      <c r="C23" s="79" t="s">
         <v>490</v>
       </c>
       <c r="E23" s="19"/>
       <c r="F23" s="19"/>
-      <c r="G23" s="82" t="s">
+      <c r="G23" s="81" t="s">
         <v>491</v>
       </c>
       <c r="H23" s="58" t="s">
         <v>191</v>
       </c>
-      <c r="I23" s="80" t="s">
+      <c r="I23" s="79" t="s">
         <v>492</v>
       </c>
-      <c r="J23" s="82" t="s">
+      <c r="J23" s="81" t="s">
         <v>22</v>
       </c>
     </row>
@@ -4056,11 +4059,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E204"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B81" sqref="B81"/>
+      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4354,7 +4357,7 @@
       <c r="A26" s="72" t="s">
         <v>453</v>
       </c>
-      <c r="B26" s="76" t="s">
+      <c r="B26" s="82" t="s">
         <v>486</v>
       </c>
       <c r="C26" s="72" t="s">
@@ -4369,7 +4372,7 @@
       <c r="A27" s="72" t="s">
         <v>453</v>
       </c>
-      <c r="B27" s="73" t="s">
+      <c r="B27" s="83" t="s">
         <v>465</v>
       </c>
       <c r="C27" s="72" t="s">
@@ -4915,10 +4918,10 @@
       <c r="A81" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="B81" s="78" t="s">
+      <c r="B81" s="77" t="s">
         <v>487</v>
       </c>
-      <c r="C81" s="79" t="s">
+      <c r="C81" s="78" t="s">
         <v>488</v>
       </c>
     </row>
@@ -5260,7 +5263,7 @@
       <c r="A116" s="33" t="s">
         <v>130</v>
       </c>
-      <c r="B116" s="77">
+      <c r="B116" s="76">
         <v>1</v>
       </c>
       <c r="C116" s="33" t="s">
@@ -5934,8 +5937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5969,7 +5972,7 @@
         <v>408</v>
       </c>
       <c r="C2" s="8">
-        <v>201708152</v>
+        <v>201708153</v>
       </c>
       <c r="D2" s="67" t="s">
         <v>410</v>

</xml_diff>

<commit_message>
Amended Form C to force leading 0s on parcel numbers
</commit_message>
<xml_diff>
--- a/Hluvukani_C_registrar_parcelas/Hluvukani_C_registrar_parcelas-media/Hluvukani_C_registrar_parcelas.xlsx
+++ b/Hluvukani_C_registrar_parcelas/Hluvukani_C_registrar_parcelas-media/Hluvukani_C_registrar_parcelas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7380" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="494">
   <si>
     <t>type</t>
   </si>
@@ -1562,14 +1562,24 @@
   <si>
     <t>Resposta invalida - O campo de nome não pode incluir um novo paragrafo. Faça a favor de eliminar qualquer linha adicional.</t>
   </si>
+  <si>
+    <t>regex(.,'[0-9]{6}')</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1801,422 +1811,427 @@
   </borders>
   <cellStyleXfs count="237">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="233" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="235" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="233" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="235" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="235" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="235" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="235" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="235" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="237">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2794,11 +2809,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P76"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="L20" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L27" sqref="L27"/>
+      <selection pane="bottomRight" activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2974,23 +2989,25 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+    <row r="9" spans="1:16" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="85" t="s">
         <v>315</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="84" t="s">
         <v>316</v>
       </c>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="J9" s="17" t="s">
+      <c r="E9" s="84"/>
+      <c r="F9" s="84"/>
+      <c r="H9" s="86" t="s">
+        <v>493</v>
+      </c>
+      <c r="J9" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="L9" s="36" t="s">
+      <c r="L9" s="86" t="s">
         <v>93</v>
       </c>
     </row>
@@ -4059,7 +4076,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E204"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -5938,7 +5955,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5972,7 +5989,7 @@
         <v>408</v>
       </c>
       <c r="C2" s="8">
-        <v>201708153</v>
+        <v>201708171</v>
       </c>
       <c r="D2" s="67" t="s">
         <v>410</v>

</xml_diff>

<commit_message>
Amends Form C with new names
</commit_message>
<xml_diff>
--- a/Hluvukani_C_registrar_parcelas/Hluvukani_C_registrar_parcelas-media/Hluvukani_C_registrar_parcelas.xlsx
+++ b/Hluvukani_C_registrar_parcelas/Hluvukani_C_registrar_parcelas-media/Hluvukani_C_registrar_parcelas.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18528"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -5971,7 +5971,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6005,7 +6005,7 @@
         <v>408</v>
       </c>
       <c r="C2" s="85">
-        <v>201710251</v>
+        <v>201711011</v>
       </c>
       <c r="D2" s="88" t="s">
         <v>410</v>

</xml_diff>

<commit_message>
Updates Form C with new names
</commit_message>
<xml_diff>
--- a/Hluvukani_C_registrar_parcelas/Hluvukani_C_registrar_parcelas-media/Hluvukani_C_registrar_parcelas.xlsx
+++ b/Hluvukani_C_registrar_parcelas/Hluvukani_C_registrar_parcelas-media/Hluvukani_C_registrar_parcelas.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18528"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\projects\illovo\ODK Forms\hluvukani-odk-forms\Hluvukani_C_registrar_parcelas\Hluvukani_C_registrar_parcelas-media\"/>
@@ -2823,6 +2823,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P76"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -4090,6 +4091,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:E204"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -5968,10 +5970,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6005,7 +6008,7 @@
         <v>408</v>
       </c>
       <c r="C2" s="85">
-        <v>201711011</v>
+        <v>2017110601</v>
       </c>
       <c r="D2" s="88" t="s">
         <v>410</v>

</xml_diff>